<commit_message>
add 5/9 stuff and update trends
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -349,6 +349,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -429,6 +432,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,6 +560,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -633,6 +642,9 @@
                   <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
@@ -759,6 +771,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -838,6 +853,9 @@
                   <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
@@ -964,6 +982,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1043,6 +1064,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1167,6 +1191,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1247,6 +1274,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1261,8 +1291,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="449187264"/>
-        <c:axId val="449187656"/>
+        <c:axId val="376111088"/>
+        <c:axId val="376111480"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1383,6 +1413,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1463,6 +1496,9 @@
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
                   <c:v>0.94482758620689655</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.96478873239436624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1477,11 +1513,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="449188440"/>
-        <c:axId val="449188048"/>
+        <c:axId val="376112264"/>
+        <c:axId val="376111872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="449187264"/>
+        <c:axId val="376111088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -1595,12 +1631,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449187656"/>
+        <c:crossAx val="376111480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="449187656"/>
+        <c:axId val="376111480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1713,12 +1749,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449187264"/>
+        <c:crossAx val="376111088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="449188048"/>
+        <c:axId val="376111872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1814,12 +1850,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449188440"/>
+        <c:crossAx val="376112264"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="449188440"/>
+        <c:axId val="376112264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="449188048"/>
+        <c:crossAx val="376111872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2100,6 +2136,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2180,6 +2219,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>42.282068966026038</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43.825352112787222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2305,6 +2347,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2385,6 +2430,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>34.999999998835847</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>36.116666675079614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2510,6 +2558,9 @@
                 <c:pt idx="23">
                   <c:v>42498</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>42499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2590,6 +2641,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>57.783333335537463</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>58.833333340007812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2604,11 +2658,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="449189224"/>
-        <c:axId val="449189616"/>
+        <c:axId val="376112656"/>
+        <c:axId val="376113048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="449189224"/>
+        <c:axId val="376112656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2722,12 +2776,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449189616"/>
+        <c:crossAx val="376113048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="449189616"/>
+        <c:axId val="376113048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2840,7 +2894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="449189224"/>
+        <c:crossAx val="376112656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4032,7 +4086,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4043,7 +4097,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="122" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4054,7 +4108,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8666189" cy="6292746"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4081,7 +4135,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8666189" cy="6292746"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4367,10 +4421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:J25"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5217,6 +5271,38 @@
         <v>57.783333335537463</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42499</v>
+      </c>
+      <c r="B26">
+        <v>142</v>
+      </c>
+      <c r="C26">
+        <v>137</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>137</v>
+      </c>
+      <c r="G26">
+        <v>0.96478873239436624</v>
+      </c>
+      <c r="H26" s="2">
+        <v>43.825352112787222</v>
+      </c>
+      <c r="I26" s="2">
+        <v>36.116666675079614</v>
+      </c>
+      <c r="J26" s="2">
+        <v>58.833333340007812</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removed duplicate 128-11 run
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wabtec\Documents\GitHub\eaglep3-reporting\EC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macosta\Documents\GitHub\eaglep3-reporting\EC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -448,7 +448,7 @@
                   <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>145</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,7 +671,7 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>141</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,7 +894,7 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>141</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1353,8 +1353,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456904200"/>
-        <c:axId val="456904592"/>
+        <c:axId val="206117168"/>
+        <c:axId val="205697848"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1572,7 +1572,7 @@
                   <c:v>0.93661971830985913</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.97241379310344822</c:v>
+                  <c:v>0.97222222222222221</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,11 +1587,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456905376"/>
-        <c:axId val="456904984"/>
+        <c:axId val="205708856"/>
+        <c:axId val="205702328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456904200"/>
+        <c:axId val="206117168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -1705,12 +1705,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456904592"/>
+        <c:crossAx val="205697848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456904592"/>
+        <c:axId val="205697848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,12 +1823,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456904200"/>
+        <c:crossAx val="206117168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456904984"/>
+        <c:axId val="205702328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1924,12 +1924,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456905376"/>
+        <c:crossAx val="205708856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456905376"/>
+        <c:axId val="205708856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1939,7 +1939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456904984"/>
+        <c:crossAx val="205702328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2307,7 +2307,7 @@
                   <c:v>43.142253521112664</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43.178160919117389</c:v>
+                  <c:v>43.391666666163864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2768,11 +2768,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456906160"/>
-        <c:axId val="456906552"/>
+        <c:axId val="206048728"/>
+        <c:axId val="206049112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456906160"/>
+        <c:axId val="206048728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2886,12 +2886,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456906552"/>
+        <c:crossAx val="206049112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456906552"/>
+        <c:axId val="206049112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3004,7 +3004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456906160"/>
+        <c:crossAx val="206048728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4196,7 +4196,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4207,7 +4207,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4218,7 +4218,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672413" cy="6294493"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4245,7 +4245,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672413" cy="6294493"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4534,7 +4534,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="H28" sqref="H28:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5450,10 +5450,10 @@
         <v>42501</v>
       </c>
       <c r="B28">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -5462,13 +5462,13 @@
         <v>4</v>
       </c>
       <c r="F28">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G28" s="9">
-        <v>0.97241379310344822</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="H28" s="2">
-        <v>43.178160919117389</v>
+        <v>43.391666666163864</v>
       </c>
       <c r="I28" s="2">
         <v>35.399999998044223</v>

</xml_diff>

<commit_message>
created reports for 5/12
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -62,8 +62,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,7 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -138,6 +139,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,6 +364,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -449,6 +456,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -583,6 +593,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -672,6 +685,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,6 +822,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -895,6 +914,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1029,6 +1051,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1117,6 +1142,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1250,6 +1278,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1339,6 +1370,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1353,8 +1387,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206117168"/>
-        <c:axId val="205697848"/>
+        <c:axId val="293812856"/>
+        <c:axId val="293814424"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1484,6 +1518,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1573,6 +1610,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.97222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.0%">
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,11 +1627,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="205708856"/>
-        <c:axId val="205702328"/>
+        <c:axId val="293809328"/>
+        <c:axId val="293809720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206117168"/>
+        <c:axId val="293812856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -1705,12 +1745,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205697848"/>
+        <c:crossAx val="293814424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205697848"/>
+        <c:axId val="293814424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,12 +1863,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206117168"/>
+        <c:crossAx val="293812856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205702328"/>
+        <c:axId val="293809720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1924,12 +1964,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205708856"/>
+        <c:crossAx val="293809328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205708856"/>
+        <c:axId val="293809328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1939,7 +1979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205702328"/>
+        <c:crossAx val="293809720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2219,6 +2259,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2308,6 +2351,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43.391666666163864</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44.467661691188411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2442,6 +2488,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2531,6 +2580,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>35.399999998044223</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34.116666658082977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2665,6 +2717,9 @@
                 <c:pt idx="26">
                   <c:v>42501</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>42502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2754,6 +2809,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>68.833333330694586</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>114.299999991199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2768,11 +2826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206048728"/>
-        <c:axId val="206049112"/>
+        <c:axId val="245151544"/>
+        <c:axId val="245153112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206048728"/>
+        <c:axId val="245151544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2886,12 +2944,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206049112"/>
+        <c:crossAx val="245153112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206049112"/>
+        <c:axId val="245153112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3004,7 +3062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206048728"/>
+        <c:crossAx val="245151544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4196,7 +4254,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4531,10 +4589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28:J28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5477,6 +5535,38 @@
         <v>68.833333330694586</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42502</v>
+      </c>
+      <c r="B29">
+        <v>141</v>
+      </c>
+      <c r="C29">
+        <v>134</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>134</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="H29" s="2">
+        <v>44.467661691188411</v>
+      </c>
+      <c r="I29" s="2">
+        <v>34.116666658082977</v>
+      </c>
+      <c r="J29" s="2">
+        <v>114.299999991199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates per discussion in the meeting.
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,7 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -137,10 +137,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1387,8 +1388,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="293812856"/>
-        <c:axId val="293814424"/>
+        <c:axId val="347600912"/>
+        <c:axId val="347601304"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1627,11 +1628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="293809328"/>
-        <c:axId val="293809720"/>
+        <c:axId val="347602088"/>
+        <c:axId val="347601696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="293812856"/>
+        <c:axId val="347600912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -1745,12 +1746,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293814424"/>
+        <c:crossAx val="347601304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293814424"/>
+        <c:axId val="347601304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1863,12 +1864,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293812856"/>
+        <c:crossAx val="347600912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293809720"/>
+        <c:axId val="347601696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1964,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293809328"/>
+        <c:crossAx val="347602088"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293809328"/>
+        <c:axId val="347602088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +1980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="293809720"/>
+        <c:crossAx val="347601696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2826,11 +2827,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="245151544"/>
-        <c:axId val="245153112"/>
+        <c:axId val="347602872"/>
+        <c:axId val="347603264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="245151544"/>
+        <c:axId val="347602872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2944,12 +2945,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245153112"/>
+        <c:crossAx val="347603264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245153112"/>
+        <c:axId val="347603264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3062,7 +3063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245151544"/>
+        <c:crossAx val="347602872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4254,7 +4255,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4276,7 +4277,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8663214" cy="6304643"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4591,8 +4592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5014,556 +5015,556 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="3">
         <v>42481</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>127</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>121</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <v>122</v>
       </c>
       <c r="G13" s="6">
         <f t="shared" si="2"/>
         <v>0.96062992125984248</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="5">
         <v>41.2875661375856</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="5">
         <v>34.016666666138917</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="5">
         <v>58.416666659759358</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="3">
         <v>42482</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>72</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>61</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>2</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>9</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="4">
         <v>63</v>
       </c>
       <c r="G14" s="6">
         <f t="shared" si="2"/>
         <v>0.875</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="5">
         <v>43.831944444682449</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="5">
         <v>36.216666667023674</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="5">
         <v>84.883333331672475</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="3">
         <v>42483</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>95</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>81</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>0</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>14</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <v>81</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" ref="G15:G22" si="3">F15/B15</f>
         <v>0.85263157894736841</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="5">
         <v>44.743508772520151</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="5">
         <v>36.400000001303852</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="5">
         <v>67.266666664509103</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="3">
         <v>42484</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>141</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>128</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>2</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>11</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="4">
         <v>130</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="6">
         <f t="shared" si="3"/>
         <v>0.92198581560283688</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="5">
         <v>43.81430260078568</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="5">
         <v>35.666666674660519</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="5">
         <v>97.066666663158685</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="3">
         <v>42485</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>40</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>38</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>0</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>38</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="6">
         <f t="shared" si="3"/>
         <v>0.95</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="5">
         <v>40.633333333495926</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="5">
         <v>36.56666666502133</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="5">
         <v>50.033333336468786</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="3">
         <v>42491</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>144</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>139</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>3</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="4">
         <v>141</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="6">
         <f t="shared" si="3"/>
         <v>0.97916666666666663</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="5">
         <v>41.443055555428145</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="5">
         <v>30.483333334559575</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="5">
         <v>49.966666664695367</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="3">
         <v>42492</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>139</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>135</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>3</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="4">
         <v>136</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="6">
         <f t="shared" si="3"/>
         <v>0.97841726618705038</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="5">
         <v>41.887889688142756</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="5">
         <v>35.749999996041879</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="5">
         <v>49.916666673962027</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="3">
         <v>42493</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>145</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>142</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>3</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="4">
         <v>142</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="6">
         <f t="shared" si="3"/>
         <v>0.97931034482758617</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="5">
         <v>42.004050925243064</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="5">
         <v>35.883333329111338</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="5">
         <v>53.433333324501291</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="3">
         <v>42494</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>145</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>141</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>4</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="4">
         <v>141</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="6">
         <f t="shared" si="3"/>
         <v>0.97241379310344822</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="5">
         <v>42.675172413760777</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="5">
         <v>35.500000000465661</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="5">
         <v>55.966666663298383</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="3">
         <v>42495</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>144</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>139</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>0</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>5</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="4">
         <v>139</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="6">
         <f t="shared" si="3"/>
         <v>0.96527777777777779</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="5">
         <v>41.983932853269792</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="5">
         <v>34.449999995995313</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="5">
         <v>53.816666663624346</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="3">
         <v>42496</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>146</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>146</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>0</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="4">
         <v>146</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <v>1</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="5">
         <v>43.054794521024768</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="5">
         <v>35.300000006100163</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="5">
         <v>57.366666665766388</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="3">
         <v>42497</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>147</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>141</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>6</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="4">
         <v>141</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>0.95918367346938771</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="5">
         <v>42.212018140387357</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="5">
         <v>35.083333330694586</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="5">
         <v>52.933333333348855</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="3">
         <v>42498</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>145</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>137</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>0</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>8</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="4">
         <v>137</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <v>0.94482758620689655</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="5">
         <v>42.282068966026038</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="5">
         <v>34.999999998835847</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="5">
         <v>57.783333335537463</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="3">
         <v>42499</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="4">
         <v>143</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>137</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>0</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="4">
         <v>6</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="4">
         <v>137</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <v>0.95804195804195802</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="5">
         <v>43.519580419690811</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="5">
         <v>36.116666675079614</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="5">
         <v>58.833333340007812</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="3">
         <v>42500</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="4">
         <v>142</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>133</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>9</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="4">
         <v>133</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <v>0.93661971830985913</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="5">
         <v>43.142253521112664</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="5">
         <v>34.983333328273147</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="5">
         <v>58.716666667023674</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="3">
         <v>42501</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4">
         <v>144</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>140</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>4</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="4">
         <v>140</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <v>0.97222222222222221</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="5">
         <v>43.391666666163864</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="5">
         <v>35.399999998044223</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="5">
         <v>68.833333330694586</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="3">
         <v>42502</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>141</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>134</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>0</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>7</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="4">
         <v>134</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="9">
         <v>0.95</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="5">
         <v>44.467661691188411</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="5">
         <v>34.116666658082977</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="5">
         <v>114.299999991199</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finally caught up from weekend
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macosta\Documents\GitHub\eaglep3-reporting\EC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu\Documents\GitHub\eaglep3-reporting\EC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -368,6 +368,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -460,6 +472,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,6 +621,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -689,6 +725,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -826,6 +874,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -918,6 +978,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1055,6 +1127,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1146,6 +1230,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1282,6 +1378,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1374,6 +1482,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1388,8 +1508,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="347600912"/>
-        <c:axId val="347601304"/>
+        <c:axId val="300825480"/>
+        <c:axId val="300825872"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1522,6 +1642,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1614,6 +1746,18 @@
                 </c:pt>
                 <c:pt idx="27" formatCode="0.0%">
                   <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>0.88811188811188813</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>0.98620689655172411</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>0.92253521126760563</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>0.95488721804511278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1628,11 +1772,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="347602088"/>
-        <c:axId val="347601696"/>
+        <c:axId val="300826656"/>
+        <c:axId val="300826264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="347600912"/>
+        <c:axId val="300825480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -1746,12 +1890,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347601304"/>
+        <c:crossAx val="300825872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347601304"/>
+        <c:axId val="300825872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,12 +2008,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347600912"/>
+        <c:crossAx val="300825480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347601696"/>
+        <c:axId val="300826264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1965,12 +2109,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347602088"/>
+        <c:crossAx val="300826656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347602088"/>
+        <c:axId val="300826656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +2124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347601696"/>
+        <c:crossAx val="300826264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2263,6 +2407,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2355,6 +2511,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>44.467661691188411</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42.152214452051197</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42.423793103425474</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42.673591549260685</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44.154761904593265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2492,6 +2660,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2584,6 +2764,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>34.116666658082977</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35.100000001257285</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34.983333338750526</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.66666666418314</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35.399999998044223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2721,6 +2913,18 @@
                 <c:pt idx="27">
                   <c:v>42502</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2813,6 +3017,18 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>114.299999991199</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>60.266666673123837</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>56.049999995157123</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>57.20000000204891</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>76.633333330973983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2827,11 +3043,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="347602872"/>
-        <c:axId val="347603264"/>
+        <c:axId val="300827440"/>
+        <c:axId val="300827832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="347602872"/>
+        <c:axId val="300827440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2945,12 +3161,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347603264"/>
+        <c:crossAx val="300827832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347603264"/>
+        <c:axId val="300827832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3063,7 +3279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347602872"/>
+        <c:crossAx val="300827440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4255,7 +4471,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4277,7 +4493,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663214" cy="6304643"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4590,10 +4806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5568,6 +5784,134 @@
         <v>114.299999991199</v>
       </c>
     </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>42503</v>
+      </c>
+      <c r="B30">
+        <v>143</v>
+      </c>
+      <c r="C30">
+        <v>127</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>127</v>
+      </c>
+      <c r="G30">
+        <v>0.88811188811188813</v>
+      </c>
+      <c r="H30" s="2">
+        <v>42.152214452051197</v>
+      </c>
+      <c r="I30" s="2">
+        <v>35.100000001257285</v>
+      </c>
+      <c r="J30" s="2">
+        <v>60.266666673123837</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>42504</v>
+      </c>
+      <c r="B31">
+        <v>145</v>
+      </c>
+      <c r="C31">
+        <v>143</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>143</v>
+      </c>
+      <c r="G31">
+        <v>0.98620689655172411</v>
+      </c>
+      <c r="H31" s="2">
+        <v>42.423793103425474</v>
+      </c>
+      <c r="I31" s="2">
+        <v>34.983333338750526</v>
+      </c>
+      <c r="J31" s="2">
+        <v>56.049999995157123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>42505</v>
+      </c>
+      <c r="B32">
+        <v>142</v>
+      </c>
+      <c r="C32">
+        <v>131</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>11</v>
+      </c>
+      <c r="F32">
+        <v>131</v>
+      </c>
+      <c r="G32">
+        <v>0.92253521126760563</v>
+      </c>
+      <c r="H32" s="2">
+        <v>42.673591549260685</v>
+      </c>
+      <c r="I32" s="2">
+        <v>35.66666666418314</v>
+      </c>
+      <c r="J32" s="2">
+        <v>57.20000000204891</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>42506</v>
+      </c>
+      <c r="B33">
+        <v>133</v>
+      </c>
+      <c r="C33">
+        <v>127</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <v>127</v>
+      </c>
+      <c r="G33">
+        <v>0.95488721804511278</v>
+      </c>
+      <c r="H33" s="2">
+        <v>44.154761904593265</v>
+      </c>
+      <c r="I33" s="2">
+        <v>35.399999998044223</v>
+      </c>
+      <c r="J33" s="2">
+        <v>76.633333330973983</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
first crack at 5/17 stuff
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -380,6 +380,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -484,6 +487,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,6 +639,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -737,6 +746,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -886,6 +898,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -990,6 +1005,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,6 +1157,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1242,6 +1263,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1390,6 +1414,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1494,6 +1521,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,8 +1538,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="300825480"/>
-        <c:axId val="300825872"/>
+        <c:axId val="294599304"/>
+        <c:axId val="294599696"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1654,6 +1684,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1758,6 +1791,9 @@
                 </c:pt>
                 <c:pt idx="31" formatCode="General">
                   <c:v>0.95488721804511278</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>0.94405594405594406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,11 +1808,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="300826656"/>
-        <c:axId val="300826264"/>
+        <c:axId val="300150232"/>
+        <c:axId val="294600088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="300825480"/>
+        <c:axId val="294599304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -1890,12 +1926,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300825872"/>
+        <c:crossAx val="294599696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300825872"/>
+        <c:axId val="294599696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,12 +2044,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300825480"/>
+        <c:crossAx val="294599304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300826264"/>
+        <c:axId val="294600088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2109,12 +2145,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300826656"/>
+        <c:crossAx val="300150232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300826656"/>
+        <c:axId val="300150232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,7 +2160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="300826264"/>
+        <c:crossAx val="294600088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2240,7 +2276,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2419,6 +2454,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2523,6 +2561,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44.154761904593265</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43.071445221369565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2672,6 +2713,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2776,6 +2820,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>35.399999998044223</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34.833333335118368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2925,6 +2972,9 @@
                 <c:pt idx="31">
                   <c:v>42506</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>42507</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3029,6 +3079,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>76.633333330973983</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>67.399999997578561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3043,11 +3096,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="300827440"/>
-        <c:axId val="300827832"/>
+        <c:axId val="300151016"/>
+        <c:axId val="300151408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="300827440"/>
+        <c:axId val="300151016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3094,7 +3147,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3161,12 +3213,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300827832"/>
+        <c:crossAx val="300151408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300827832"/>
+        <c:axId val="300151408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3212,7 +3264,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3279,7 +3330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300827440"/>
+        <c:crossAx val="300151016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3293,7 +3344,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4471,7 +4521,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4493,7 +4543,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8680739" cy="6299489"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4806,10 +4856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:J30"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5912,6 +5962,38 @@
         <v>76.633333330973983</v>
       </c>
     </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42507</v>
+      </c>
+      <c r="B34">
+        <v>143</v>
+      </c>
+      <c r="C34">
+        <v>135</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <v>135</v>
+      </c>
+      <c r="G34">
+        <v>0.94405594405594406</v>
+      </c>
+      <c r="H34" s="2">
+        <v>43.071445221369565</v>
+      </c>
+      <c r="I34" s="2">
+        <v>34.833333335118368</v>
+      </c>
+      <c r="J34" s="2">
+        <v>67.399999997578561</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update all missing trips
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -392,6 +392,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -505,6 +514,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -663,6 +681,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -776,6 +803,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -934,6 +970,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1047,6 +1092,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1205,6 +1259,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1318,6 +1381,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1474,6 +1546,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1587,6 +1668,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,8 +1691,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="327166352"/>
-        <c:axId val="327167136"/>
+        <c:axId val="258090528"/>
+        <c:axId val="352458064"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1756,6 +1846,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1869,6 +1968,15 @@
                 </c:pt>
                 <c:pt idx="34" formatCode="General">
                   <c:v>0.91111111111111109</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>0.94927536231884058</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>0.89928057553956831</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>0.93076923076923079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,11 +1991,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="327167920"/>
-        <c:axId val="327167528"/>
+        <c:axId val="352458848"/>
+        <c:axId val="352458456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="327166352"/>
+        <c:axId val="258090528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2001,12 +2109,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327167136"/>
+        <c:crossAx val="352458064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327167136"/>
+        <c:axId val="352458064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2119,12 +2227,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327166352"/>
+        <c:crossAx val="258090528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327167528"/>
+        <c:axId val="352458456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2220,12 +2328,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327167920"/>
+        <c:crossAx val="352458848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327167920"/>
+        <c:axId val="352458848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2235,7 +2343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327167528"/>
+        <c:crossAx val="352458456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2539,6 +2647,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2652,6 +2769,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>42.520864197882581</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44.964734298409894</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45.517146282958322</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44.905000000228533</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2810,6 +2936,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2923,6 +3058,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>35.399999998044223</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34.516666667768732</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.033333332743496</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>35.216666663764045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3081,6 +3225,15 @@
                 <c:pt idx="34">
                   <c:v>42509</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>42510</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42511</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42512</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3194,6 +3347,15 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>61.166666663484648</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>63.233333331299946</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>126.35000000009313</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>65.900000003166497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3208,11 +3370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="327168704"/>
-        <c:axId val="327169096"/>
+        <c:axId val="352459632"/>
+        <c:axId val="352460024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="327168704"/>
+        <c:axId val="352459632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3326,12 +3488,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327169096"/>
+        <c:crossAx val="352460024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327169096"/>
+        <c:axId val="352460024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3444,7 +3606,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327168704"/>
+        <c:crossAx val="352459632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4636,7 +4798,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4658,7 +4820,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8671560" cy="6294120"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4971,15 +5133,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H39" sqref="H39:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -6173,6 +6335,102 @@
         <v>61.166666663484648</v>
       </c>
     </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>42510</v>
+      </c>
+      <c r="B37">
+        <v>138</v>
+      </c>
+      <c r="C37">
+        <v>130</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>131</v>
+      </c>
+      <c r="G37">
+        <v>0.94927536231884058</v>
+      </c>
+      <c r="H37" s="2">
+        <v>44.964734298409894</v>
+      </c>
+      <c r="I37" s="2">
+        <v>34.516666667768732</v>
+      </c>
+      <c r="J37" s="2">
+        <v>63.233333331299946</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>42511</v>
+      </c>
+      <c r="B38">
+        <v>139</v>
+      </c>
+      <c r="C38">
+        <v>125</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>14</v>
+      </c>
+      <c r="F38">
+        <v>125</v>
+      </c>
+      <c r="G38">
+        <v>0.89928057553956831</v>
+      </c>
+      <c r="H38" s="2">
+        <v>45.517146282958322</v>
+      </c>
+      <c r="I38" s="2">
+        <v>36.033333332743496</v>
+      </c>
+      <c r="J38" s="2">
+        <v>126.35000000009313</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>42512</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+      <c r="C39">
+        <v>121</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>121</v>
+      </c>
+      <c r="G39">
+        <v>0.93076923076923079</v>
+      </c>
+      <c r="H39" s="2">
+        <v>44.905000000228533</v>
+      </c>
+      <c r="I39" s="2">
+        <v>35.216666663764045</v>
+      </c>
+      <c r="J39" s="2">
+        <v>65.900000003166497</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fill in rest of details
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -401,6 +401,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -523,6 +526,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -690,6 +696,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -812,6 +821,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,6 +991,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1101,6 +1116,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,6 +1286,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1389,6 +1410,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1555,6 +1579,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1677,6 +1704,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1691,8 +1721,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="258090528"/>
-        <c:axId val="352458064"/>
+        <c:axId val="164320192"/>
+        <c:axId val="164320584"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1855,6 +1885,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1977,6 +2010,9 @@
                 </c:pt>
                 <c:pt idx="37" formatCode="General">
                   <c:v>0.93076923076923079</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>0.93939393939393945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1991,11 +2027,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="352458848"/>
-        <c:axId val="352458456"/>
+        <c:axId val="164321368"/>
+        <c:axId val="164320976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="258090528"/>
+        <c:axId val="164320192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2109,12 +2145,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352458064"/>
+        <c:crossAx val="164320584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352458064"/>
+        <c:axId val="164320584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,12 +2263,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258090528"/>
+        <c:crossAx val="164320192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352458456"/>
+        <c:axId val="164320976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2328,12 +2364,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352458848"/>
+        <c:crossAx val="164321368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352458848"/>
+        <c:axId val="164321368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="352458456"/>
+        <c:crossAx val="164320976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2459,7 +2495,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2656,6 +2691,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2778,6 +2816,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>44.905000000228533</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>45.650378787990618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2945,6 +2986,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3067,6 +3111,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>35.216666663764045</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>35.516666660550982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3234,6 +3281,9 @@
                 <c:pt idx="37">
                   <c:v>42512</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>42513</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3356,6 +3406,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>65.900000003166497</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>143.45000000554137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3370,11 +3423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="352459632"/>
-        <c:axId val="352460024"/>
+        <c:axId val="164322152"/>
+        <c:axId val="164322544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="352459632"/>
+        <c:axId val="164322152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3421,7 +3474,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3488,12 +3540,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352460024"/>
+        <c:crossAx val="164322544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352460024"/>
+        <c:axId val="164322544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3539,7 +3591,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3606,7 +3657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352459632"/>
+        <c:crossAx val="164322152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3620,7 +3671,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4798,7 +4848,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4820,7 +4870,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8671560" cy="6294120"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5133,10 +5183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39:J39"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6431,6 +6481,38 @@
         <v>65.900000003166497</v>
       </c>
     </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>42513</v>
+      </c>
+      <c r="B40">
+        <v>132</v>
+      </c>
+      <c r="C40">
+        <v>124</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>124</v>
+      </c>
+      <c r="G40">
+        <v>0.93939393939393945</v>
+      </c>
+      <c r="H40" s="2">
+        <v>45.650378787990618</v>
+      </c>
+      <c r="I40" s="2">
+        <v>35.516666660550982</v>
+      </c>
+      <c r="J40" s="2">
+        <v>143.45000000554137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates for 24th. also add 25th just for a quick look
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -404,6 +404,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -529,6 +532,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,6 +705,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -824,6 +833,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,6 +1006,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1119,6 +1134,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1289,6 +1307,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1414,6 +1435,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1582,6 +1606,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1707,6 +1734,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,8 +1751,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164320192"/>
-        <c:axId val="164320584"/>
+        <c:axId val="244363544"/>
+        <c:axId val="390204272"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1888,6 +1918,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2013,6 +2046,9 @@
                 </c:pt>
                 <c:pt idx="38" formatCode="General">
                   <c:v>0.93939393939393945</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>0.78632478632478631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2027,11 +2063,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164321368"/>
-        <c:axId val="164320976"/>
+        <c:axId val="390205056"/>
+        <c:axId val="390204664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="164320192"/>
+        <c:axId val="244363544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2145,12 +2181,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164320584"/>
+        <c:crossAx val="390204272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164320584"/>
+        <c:axId val="390204272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2263,12 +2299,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164320192"/>
+        <c:crossAx val="244363544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164320976"/>
+        <c:axId val="390204664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2364,12 +2400,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164321368"/>
+        <c:crossAx val="390205056"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164321368"/>
+        <c:axId val="390205056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,7 +2415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164320976"/>
+        <c:crossAx val="390204664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2495,6 +2531,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2694,6 +2731,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2819,6 +2859,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>45.650378787990618</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42.115099714529642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2989,6 +3032,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3114,6 +3160,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>35.516666660550982</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>25.833333337213844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3284,6 +3333,9 @@
                 <c:pt idx="38">
                   <c:v>42513</c:v>
                 </c:pt>
+                <c:pt idx="39">
+                  <c:v>42514</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3409,6 +3461,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>143.45000000554137</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>193.56666667386889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3423,11 +3478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164322152"/>
-        <c:axId val="164322544"/>
+        <c:axId val="390205840"/>
+        <c:axId val="246009888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="164322152"/>
+        <c:axId val="390205840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3474,6 +3529,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3540,12 +3596,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164322544"/>
+        <c:crossAx val="246009888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164322544"/>
+        <c:axId val="246009888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,6 +3647,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3657,7 +3714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164322152"/>
+        <c:crossAx val="390205840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3671,6 +3728,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4848,7 +4906,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5183,10 +5241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H41" sqref="H41:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6513,6 +6571,38 @@
         <v>143.45000000554137</v>
       </c>
     </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42514</v>
+      </c>
+      <c r="B41">
+        <v>117</v>
+      </c>
+      <c r="C41">
+        <v>91</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>25</v>
+      </c>
+      <c r="F41">
+        <v>92</v>
+      </c>
+      <c r="G41">
+        <v>0.78632478632478631</v>
+      </c>
+      <c r="H41" s="2">
+        <v>42.115099714529642</v>
+      </c>
+      <c r="I41" s="2">
+        <v>25.833333337213844</v>
+      </c>
+      <c r="J41" s="2">
+        <v>193.56666667386889</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
additions from the 05/27th to the 06/6th
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu\Documents\GitHub\eaglep3-reporting\EC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wabtec\Documents\GitHub\eaglep3-reporting\EC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -90,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -113,12 +113,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -143,9 +163,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,6 +445,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -547,6 +612,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,6 +824,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -860,6 +991,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1039,6 +1203,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1173,6 +1370,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,6 +1582,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1485,6 +1748,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1663,6 +1959,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1797,6 +2126,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1811,8 +2173,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="351659648"/>
-        <c:axId val="351660040"/>
+        <c:axId val="475704504"/>
+        <c:axId val="475704896"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1987,6 +2349,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2121,6 +2516,39 @@
                 </c:pt>
                 <c:pt idx="41" formatCode="General">
                   <c:v>0.96350364963503654</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.0%">
+                  <c:v>0.94444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>0.9452054794520548</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
+                  <c:v>0.97916666666666663</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>0.900709219858156</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>0.94160583941605835</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>0.97222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.0%">
+                  <c:v>0.92361111111111116</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.0%">
+                  <c:v>0.94444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.0%">
+                  <c:v>0.93150684931506844</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.0%">
+                  <c:v>0.95833333333333337</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.0%">
+                  <c:v>0.9375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2135,11 +2563,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256913384"/>
-        <c:axId val="256912992"/>
+        <c:axId val="475705680"/>
+        <c:axId val="475705288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="351659648"/>
+        <c:axId val="475704504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -2253,12 +2681,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351660040"/>
+        <c:crossAx val="475704896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="351660040"/>
+        <c:axId val="475704896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2371,12 +2799,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351659648"/>
+        <c:crossAx val="475704504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256912992"/>
+        <c:axId val="475705288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2472,12 +2900,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256913384"/>
+        <c:crossAx val="475705680"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256913384"/>
+        <c:axId val="475705680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2915,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256912992"/>
+        <c:crossAx val="475705288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2812,6 +3240,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2946,6 +3407,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>43.590404041090302</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.309558823504418</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.170289855177067</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42.745035461080754</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44.086614173056013</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44.44082687376067</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42.616666667529252</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00">
+                  <c:v>44.325814535981394</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00">
+                  <c:v>43.779135802217446</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00">
+                  <c:v>44.619362745562448</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.00">
+                  <c:v>43.450362318519339</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.00">
+                  <c:v>44.205845771591989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3125,6 +3619,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3259,6 +3786,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>35.899999999674037</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>36.333333329530433</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35.550000001676381</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>35.866666669026017</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>34.899999996414408</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>35.66666666418314</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>34.500000007683411</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00">
+                  <c:v>35.983333331532776</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00">
+                  <c:v>36.58333333558403</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00">
+                  <c:v>37.183333329157904</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.00">
+                  <c:v>10.833333330228925</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.00">
+                  <c:v>35.283333335537463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3438,6 +3998,39 @@
                 <c:pt idx="41">
                   <c:v>42516</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>42517</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42520</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42521</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42523</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42524</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42525</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3572,6 +4165,39 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>59.800000002142042</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>55.783333329018205</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>156.43333332496695</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>53.766666672891006</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>60.683333342894912</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>85.833333333721384</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>54.966666660038754</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.00">
+                  <c:v>57.300000004470348</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.00">
+                  <c:v>54.883333338657394</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.00">
+                  <c:v>63.200000000651926</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.00">
+                  <c:v>64.333333326503634</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.00">
+                  <c:v>64.966666671680287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3586,11 +4212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257752104"/>
-        <c:axId val="347935208"/>
+        <c:axId val="475706464"/>
+        <c:axId val="475706856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257752104"/>
+        <c:axId val="475706464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3704,12 +4330,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347935208"/>
+        <c:crossAx val="475706856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347935208"/>
+        <c:axId val="475706856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3822,7 +4448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257752104"/>
+        <c:crossAx val="475706464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5014,7 +5640,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5025,7 +5651,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5036,7 +5662,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8658311" cy="6281351"/>
+    <xdr:ext cx="8665602" cy="6287932"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5063,7 +5689,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8658311" cy="6281351"/>
+    <xdr:ext cx="8668435" cy="6290612"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5349,10 +5975,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43:J43"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8" ySplit="23" topLeftCell="I39" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="H54" sqref="H54:J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6331,31 +6960,31 @@
       <c r="A30" s="3">
         <v>42503</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="4">
         <v>143</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="4">
         <v>127</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="4">
         <v>0</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="4">
         <v>16</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="4">
         <v>127</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="4">
         <v>0.88811188811188813</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="5">
         <v>42.152214452051197</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="5">
         <v>35.100000001257285</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="5">
         <v>60.266666673123837</v>
       </c>
     </row>
@@ -6363,31 +6992,31 @@
       <c r="A31" s="3">
         <v>42504</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="4">
         <v>145</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="4">
         <v>143</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="4">
         <v>0</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="4">
         <v>2</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="4">
         <v>143</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="4">
         <v>0.98620689655172411</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="5">
         <v>42.423793103425474</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="5">
         <v>34.983333338750526</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="5">
         <v>56.049999995157123</v>
       </c>
     </row>
@@ -6395,31 +7024,31 @@
       <c r="A32" s="3">
         <v>42505</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="4">
         <v>142</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="4">
         <v>131</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="4">
         <v>0</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="4">
         <v>11</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="4">
         <v>131</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="4">
         <v>0.92253521126760563</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="5">
         <v>42.673591549260685</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I32" s="5">
         <v>35.66666666418314</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="5">
         <v>57.20000000204891</v>
       </c>
     </row>
@@ -6427,352 +7056,704 @@
       <c r="A33" s="3">
         <v>42506</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="4">
         <v>133</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="4">
         <v>127</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="4">
         <v>0</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="4">
         <v>6</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="4">
         <v>127</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="4">
         <v>0.95488721804511278</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="5">
         <v>44.154761904593265</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="5">
         <v>35.399999998044223</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J33" s="5">
         <v>76.633333330973983</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="A34" s="3">
         <v>42507</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="4">
         <v>143</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="4">
         <v>135</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="4">
         <v>0</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="4">
         <v>8</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="4">
         <v>135</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="4">
         <v>0.94405594405594406</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="5">
         <v>43.071445221369565</v>
       </c>
-      <c r="I34" s="11">
+      <c r="I34" s="5">
         <v>34.833333335118368</v>
       </c>
-      <c r="J34" s="11">
+      <c r="J34" s="5">
         <v>67.399999997578561</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
+      <c r="A35" s="3">
         <v>42508</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="4">
         <v>133</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="4">
         <v>127</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="4">
         <v>0</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="4">
         <v>6</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="4">
         <v>127</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="4">
         <v>0.95488721804511278</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="5">
         <v>44.217167919802769</v>
       </c>
-      <c r="I35" s="11">
+      <c r="I35" s="5">
         <v>35.550000001676381</v>
       </c>
-      <c r="J35" s="11">
+      <c r="J35" s="5">
         <v>67.416666668141261</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
+      <c r="A36" s="3">
         <v>42509</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="4">
         <v>135</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="4">
         <v>122</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="4">
         <v>1</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="4">
         <v>12</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="4">
         <v>123</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="4">
         <v>0.91111111111111109</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="5">
         <v>42.520864197882581</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="5">
         <v>35.399999998044223</v>
       </c>
-      <c r="J36" s="11">
+      <c r="J36" s="5">
         <v>61.166666663484648</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
+      <c r="A37" s="3">
         <v>42510</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="4">
         <v>138</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="4">
         <v>130</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="4">
         <v>7</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="4">
         <v>131</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="4">
         <v>0.94927536231884058</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="5">
         <v>44.964734298409894</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="5">
         <v>34.516666667768732</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="5">
         <v>63.233333331299946</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
+      <c r="A38" s="3">
         <v>42511</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="4">
         <v>139</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="4">
         <v>125</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="4">
         <v>0</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>14</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="4">
         <v>125</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="4">
         <v>0.89928057553956831</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="5">
         <v>45.517146282958322</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="5">
         <v>36.033333332743496</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="5">
         <v>126.35000000009313</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
+      <c r="A39" s="3">
         <v>42512</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="4">
         <v>130</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="4">
         <v>121</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="4">
         <v>0</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="4">
         <v>9</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="4">
         <v>121</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="4">
         <v>0.93076923076923079</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="5">
         <v>44.905000000228533</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="5">
         <v>35.216666663764045</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="5">
         <v>65.900000003166497</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
+      <c r="A40" s="3">
         <v>42513</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="4">
         <v>132</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="4">
         <v>124</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="4">
         <v>0</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="4">
         <v>8</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="4">
         <v>124</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="4">
         <v>0.93939393939393945</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="5">
         <v>45.650378787990618</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="5">
         <v>35.516666660550982</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="5">
         <v>143.45000000554137</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="3">
         <v>42514</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="4">
         <v>117</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="4">
         <v>91</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="4">
         <v>1</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>25</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="4">
         <v>92</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="4">
         <v>0.78632478632478631</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="5">
         <v>42.115099714529642</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="5">
         <v>25.833333337213844</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="5">
         <v>193.56666667386889</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
+      <c r="A42" s="3">
         <v>42515</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="4">
         <v>144</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="4">
         <v>117</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="4">
         <v>0</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="4">
         <v>27</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="4">
         <v>117</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="4">
         <v>0.8125</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="5">
         <v>43.560398861121101</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="5">
         <v>35.650000004097819</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="5">
         <v>55.933333332650363</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="3">
         <v>42516</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="4">
         <v>137</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="4">
         <v>132</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="4">
         <v>0</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="4">
         <v>5</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="4">
         <v>132</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="4">
         <v>0.96350364963503654</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="5">
         <v>43.590404041090302</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="5">
         <v>35.899999999674037</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="5">
         <v>59.800000002142042</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>42517</v>
+      </c>
+      <c r="B44" s="10">
+        <v>144</v>
+      </c>
+      <c r="C44" s="10">
+        <v>136</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>8</v>
+      </c>
+      <c r="F44" s="10">
+        <v>136</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="H44" s="5">
+        <v>43.309558823504418</v>
+      </c>
+      <c r="I44" s="5">
+        <v>36.333333329530433</v>
+      </c>
+      <c r="J44" s="5">
+        <v>55.783333329018205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>42518</v>
+      </c>
+      <c r="B45" s="4">
+        <v>146</v>
+      </c>
+      <c r="C45" s="4">
+        <v>138</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>8</v>
+      </c>
+      <c r="F45" s="4">
+        <v>138</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.9452054794520548</v>
+      </c>
+      <c r="H45" s="5">
+        <v>44.170289855177067</v>
+      </c>
+      <c r="I45" s="5">
+        <v>35.550000001676381</v>
+      </c>
+      <c r="J45" s="5">
+        <v>156.43333332496695</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>42519</v>
+      </c>
+      <c r="B46" s="4">
+        <v>144</v>
+      </c>
+      <c r="C46" s="4">
+        <v>141</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4">
+        <v>3</v>
+      </c>
+      <c r="F46" s="4">
+        <v>141</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="H46" s="5">
+        <v>42.745035461080754</v>
+      </c>
+      <c r="I46" s="5">
+        <v>35.866666669026017</v>
+      </c>
+      <c r="J46" s="5">
+        <v>53.766666672891006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>42520</v>
+      </c>
+      <c r="B47" s="4">
+        <v>141</v>
+      </c>
+      <c r="C47" s="4">
+        <v>127</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>14</v>
+      </c>
+      <c r="F47" s="4">
+        <v>127</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.900709219858156</v>
+      </c>
+      <c r="H47" s="5">
+        <v>44.086614173056013</v>
+      </c>
+      <c r="I47" s="5">
+        <v>34.899999996414408</v>
+      </c>
+      <c r="J47" s="5">
+        <v>60.683333342894912</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>42521</v>
+      </c>
+      <c r="B48" s="4">
+        <v>137</v>
+      </c>
+      <c r="C48" s="4">
+        <v>129</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4">
+        <v>8</v>
+      </c>
+      <c r="F48" s="4">
+        <v>129</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0.94160583941605835</v>
+      </c>
+      <c r="H48" s="5">
+        <v>44.44082687376067</v>
+      </c>
+      <c r="I48" s="5">
+        <v>35.66666666418314</v>
+      </c>
+      <c r="J48" s="5">
+        <v>85.833333333721384</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>42522</v>
+      </c>
+      <c r="B49" s="4">
+        <v>144</v>
+      </c>
+      <c r="C49" s="4">
+        <v>140</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <v>4</v>
+      </c>
+      <c r="F49" s="4">
+        <v>140</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="H49" s="5">
+        <v>42.616666667529252</v>
+      </c>
+      <c r="I49" s="5">
+        <v>34.500000007683411</v>
+      </c>
+      <c r="J49" s="5">
+        <v>54.966666660038754</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>42523</v>
+      </c>
+      <c r="B50" s="11">
+        <v>144</v>
+      </c>
+      <c r="C50" s="11">
+        <v>133</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="11">
+        <v>11</v>
+      </c>
+      <c r="F50" s="11">
+        <v>133</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="H50" s="13">
+        <v>44.325814535981394</v>
+      </c>
+      <c r="I50" s="13">
+        <v>35.983333331532776</v>
+      </c>
+      <c r="J50" s="14">
+        <v>57.300000004470348</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>42524</v>
+      </c>
+      <c r="B51" s="11">
+        <v>144</v>
+      </c>
+      <c r="C51" s="11">
+        <v>136</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11">
+        <v>8</v>
+      </c>
+      <c r="F51" s="11">
+        <v>136</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="H51" s="13">
+        <v>43.779135802217446</v>
+      </c>
+      <c r="I51" s="13">
+        <v>36.58333333558403</v>
+      </c>
+      <c r="J51" s="14">
+        <v>54.883333338657394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>42525</v>
+      </c>
+      <c r="B52" s="11">
+        <v>146</v>
+      </c>
+      <c r="C52" s="11">
+        <v>136</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="11">
+        <v>10</v>
+      </c>
+      <c r="F52" s="11">
+        <v>136</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0.93150684931506844</v>
+      </c>
+      <c r="H52" s="13">
+        <v>44.619362745562448</v>
+      </c>
+      <c r="I52" s="13">
+        <v>37.183333329157904</v>
+      </c>
+      <c r="J52" s="14">
+        <v>63.200000000651926</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>42526</v>
+      </c>
+      <c r="B53" s="11">
+        <v>144</v>
+      </c>
+      <c r="C53" s="11">
+        <v>138</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="11">
+        <v>6</v>
+      </c>
+      <c r="F53" s="11">
+        <v>138</v>
+      </c>
+      <c r="G53" s="12">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="H53" s="13">
+        <v>43.450362318519339</v>
+      </c>
+      <c r="I53" s="13">
+        <v>10.833333330228925</v>
+      </c>
+      <c r="J53" s="14">
+        <v>64.333333326503634</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>42527</v>
+      </c>
+      <c r="B54" s="11">
+        <v>144</v>
+      </c>
+      <c r="C54" s="11">
+        <v>135</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0</v>
+      </c>
+      <c r="E54" s="11">
+        <v>9</v>
+      </c>
+      <c r="F54" s="11">
+        <v>135</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0.9375</v>
+      </c>
+      <c r="H54" s="13">
+        <v>44.205845771591989</v>
+      </c>
+      <c r="I54" s="13">
+        <v>35.283333335537463</v>
+      </c>
+      <c r="J54" s="14">
+        <v>64.966666671680287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest runs as of the 23rd
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -478,6 +478,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -690,6 +693,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -947,6 +953,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1159,6 +1168,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,6 +1428,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1628,6 +1643,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1885,6 +1903,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2096,6 +2117,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2352,6 +2376,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2564,6 +2591,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2578,8 +2608,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227849832"/>
-        <c:axId val="227850224"/>
+        <c:axId val="308892480"/>
+        <c:axId val="308892872"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2832,6 +2862,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3044,6 +3077,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.78832116788321172</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.88732394366197187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3058,11 +3094,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="526206360"/>
-        <c:axId val="526205968"/>
+        <c:axId val="308893656"/>
+        <c:axId val="308893264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227849832"/>
+        <c:axId val="308892480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3176,12 +3212,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227850224"/>
+        <c:crossAx val="308892872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227850224"/>
+        <c:axId val="308892872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3294,12 +3330,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227849832"/>
+        <c:crossAx val="308892480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="526205968"/>
+        <c:axId val="308893264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3395,12 +3431,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526206360"/>
+        <c:crossAx val="308893656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="526206360"/>
+        <c:axId val="308893656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3410,7 +3446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526205968"/>
+        <c:crossAx val="308893264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3813,6 +3849,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4025,6 +4064,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>45.62978395008637</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44.351851851845694</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4282,6 +4324,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4494,6 +4539,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>36.333333329530433</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>35.966666660970077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4751,6 +4799,9 @@
                 <c:pt idx="67">
                   <c:v>42542</c:v>
                 </c:pt>
+                <c:pt idx="68">
+                  <c:v>42543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4963,6 +5014,9 @@
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>61.383333338890225</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>56.366666662506759</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4977,11 +5031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="526207144"/>
-        <c:axId val="526207536"/>
+        <c:axId val="308894440"/>
+        <c:axId val="308894832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="526207144"/>
+        <c:axId val="308894440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -5095,12 +5149,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526207536"/>
+        <c:crossAx val="308894832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="526207536"/>
+        <c:axId val="308894832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5213,7 +5267,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526207144"/>
+        <c:crossAx val="308894440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6405,7 +6459,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6416,7 +6470,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6427,7 +6481,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665602" cy="6287932"/>
+    <xdr:ext cx="8668435" cy="6290612"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6454,7 +6508,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665602" cy="6287932"/>
+    <xdr:ext cx="8668435" cy="6290612"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6740,13 +6794,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="23" topLeftCell="I54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="I64" sqref="I64"/>
+      <selection pane="bottomRight" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9058,6 +9112,40 @@
         <v>61.383333338890225</v>
       </c>
     </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>42543</v>
+      </c>
+      <c r="B70" s="4">
+        <v>142</v>
+      </c>
+      <c r="C70" s="4">
+        <v>126</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+      <c r="E70" s="4">
+        <v>16</v>
+      </c>
+      <c r="F70" s="4">
+        <f t="shared" ref="F70" si="11">C70</f>
+        <v>126</v>
+      </c>
+      <c r="G70" s="6">
+        <f t="shared" ref="G70" si="12">F70/B70</f>
+        <v>0.88732394366197187</v>
+      </c>
+      <c r="H70" s="5">
+        <v>44.351851851845694</v>
+      </c>
+      <c r="I70" s="5">
+        <v>35.966666660970077</v>
+      </c>
+      <c r="J70" s="5">
+        <v>56.366666662506759</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates from 7/10 thru 7/14
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -596,6 +596,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -862,6 +898,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1173,6 +1224,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1439,6 +1526,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1750,6 +1852,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2016,6 +2154,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2327,6 +2480,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2592,6 +2781,21 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2902,6 +3106,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3168,6 +3408,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3182,8 +3437,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326001904"/>
-        <c:axId val="327523216"/>
+        <c:axId val="347605392"/>
+        <c:axId val="347605784"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3490,6 +3745,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3756,6 +4047,21 @@
                 </c:pt>
                 <c:pt idx="85" formatCode="General">
                   <c:v>0.95804195804195802</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="General">
+                  <c:v>0.92907801418439717</c:v>
+                </c:pt>
+                <c:pt idx="87" formatCode="General">
+                  <c:v>0.90344827586206899</c:v>
+                </c:pt>
+                <c:pt idx="88" formatCode="General">
+                  <c:v>0.91970802919708028</c:v>
+                </c:pt>
+                <c:pt idx="89" formatCode="General">
+                  <c:v>0.97241379310344822</c:v>
+                </c:pt>
+                <c:pt idx="90" formatCode="General">
+                  <c:v>0.94244604316546765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3770,11 +4076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="327524000"/>
-        <c:axId val="327523608"/>
+        <c:axId val="347606568"/>
+        <c:axId val="347606176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326001904"/>
+        <c:axId val="347605392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -3888,12 +4194,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327523216"/>
+        <c:crossAx val="347605784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327523216"/>
+        <c:axId val="347605784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4006,12 +4312,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326001904"/>
+        <c:crossAx val="347605392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327523608"/>
+        <c:axId val="347606176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4107,12 +4413,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327524000"/>
+        <c:crossAx val="347606568"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327524000"/>
+        <c:axId val="347606568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4122,7 +4428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327523608"/>
+        <c:crossAx val="347606176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4238,7 +4544,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4579,6 +4884,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4845,6 +5186,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>41.913519813638452</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="0">
+                  <c:v>43.312411347968862</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43.382068964925693</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>43.175661375696237</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42.63965517234314</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42.303435113831988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5156,6 +5512,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5422,6 +5814,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>35.150000002468005</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="0">
+                  <c:v>35.866666658548638</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>35.61666666297242</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>34.599999999627471</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>35.216666663764045</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>35.283333335537463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5733,6 +6140,42 @@
                 <c:pt idx="85">
                   <c:v>42560</c:v>
                 </c:pt>
+                <c:pt idx="86">
+                  <c:v>42561</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>42562</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>42563</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>42564</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>42565</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>42566</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>42567</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>42568</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>42569</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42570</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>42571</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>42572</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5999,6 +6442,21 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>55.34999999916181</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="0">
+                  <c:v>60.066666668280959</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>55.083333333022892</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>55.533333333441988</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>55.000000001164153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6013,11 +6471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="327524784"/>
-        <c:axId val="327525176"/>
+        <c:axId val="347607352"/>
+        <c:axId val="347607744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="327524784"/>
+        <c:axId val="347607352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -6064,7 +6522,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6131,12 +6588,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327525176"/>
+        <c:crossAx val="347607744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327525176"/>
+        <c:axId val="347607744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6182,7 +6639,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6249,7 +6705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327524784"/>
+        <c:crossAx val="347607352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6263,7 +6719,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7441,7 +7896,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7452,7 +7907,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7463,7 +7918,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8671560" cy="6294120"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7490,7 +7945,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8671560" cy="6294120"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7776,10 +8231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92:J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10417,7 +10872,7 @@
     </row>
     <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <f t="shared" ref="A77:A90" si="13">A76+1</f>
+        <f t="shared" ref="A77:A110" si="13">A76+1</f>
         <v>42550</v>
       </c>
       <c r="B77">
@@ -10747,7 +11202,7 @@
         <v>57.883333337958902</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <f t="shared" si="13"/>
         <v>42560</v>
@@ -10780,14 +11235,278 @@
         <v>55.34999999916181</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
+    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <f t="shared" si="13"/>
+        <v>42561</v>
+      </c>
+      <c r="B88">
+        <v>141</v>
+      </c>
+      <c r="C88">
+        <v>131</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+      <c r="F88">
+        <v>131</v>
+      </c>
+      <c r="G88">
+        <v>0.92907801418439717</v>
+      </c>
+      <c r="H88" s="13">
+        <v>43.312411347968862</v>
+      </c>
+      <c r="I88" s="14">
+        <v>35.866666658548638</v>
+      </c>
+      <c r="J88" s="12">
+        <v>60.066666668280959</v>
+      </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
+      <c r="A89" s="3">
+        <f t="shared" si="13"/>
+        <v>42562</v>
+      </c>
+      <c r="B89">
+        <v>145</v>
+      </c>
+      <c r="C89">
+        <v>131</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>14</v>
+      </c>
+      <c r="F89">
+        <v>131</v>
+      </c>
+      <c r="G89">
+        <v>0.90344827586206899</v>
+      </c>
+      <c r="H89" s="2">
+        <v>43.382068964925693</v>
+      </c>
+      <c r="I89" s="2">
+        <v>35.61666666297242</v>
+      </c>
+      <c r="J89" s="2">
+        <v>58</v>
+      </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
+      <c r="A90" s="3">
+        <f t="shared" si="13"/>
+        <v>42563</v>
+      </c>
+      <c r="B90">
+        <v>137</v>
+      </c>
+      <c r="C90">
+        <v>126</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+      <c r="F90">
+        <v>126</v>
+      </c>
+      <c r="G90">
+        <v>0.91970802919708028</v>
+      </c>
+      <c r="H90" s="2">
+        <v>43.175661375696237</v>
+      </c>
+      <c r="I90" s="2">
+        <v>34.599999999627471</v>
+      </c>
+      <c r="J90" s="2">
+        <v>55.083333333022892</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <f t="shared" si="13"/>
+        <v>42564</v>
+      </c>
+      <c r="B91">
+        <v>145</v>
+      </c>
+      <c r="C91">
+        <v>141</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>4</v>
+      </c>
+      <c r="F91">
+        <v>141</v>
+      </c>
+      <c r="G91">
+        <v>0.97241379310344822</v>
+      </c>
+      <c r="H91" s="2">
+        <v>42.63965517234314</v>
+      </c>
+      <c r="I91" s="2">
+        <v>35.216666663764045</v>
+      </c>
+      <c r="J91" s="2">
+        <v>55.533333333441988</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <f t="shared" si="13"/>
+        <v>42565</v>
+      </c>
+      <c r="B92">
+        <v>139</v>
+      </c>
+      <c r="C92">
+        <v>131</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>8</v>
+      </c>
+      <c r="F92">
+        <v>131</v>
+      </c>
+      <c r="G92">
+        <v>0.94244604316546765</v>
+      </c>
+      <c r="H92" s="2">
+        <v>42.303435113831988</v>
+      </c>
+      <c r="I92" s="2">
+        <v>35.283333335537463</v>
+      </c>
+      <c r="J92" s="2">
+        <v>55.000000001164153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <f t="shared" si="13"/>
+        <v>42566</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <f t="shared" si="13"/>
+        <v>42567</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <f t="shared" si="13"/>
+        <v>42568</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <f t="shared" si="13"/>
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <f t="shared" si="13"/>
+        <v>42570</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <f t="shared" si="13"/>
+        <v>42571</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <f t="shared" si="13"/>
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <f t="shared" si="13"/>
+        <v>42573</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <f t="shared" si="13"/>
+        <v>42574</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <f t="shared" si="13"/>
+        <v>42575</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <f t="shared" si="13"/>
+        <v>42576</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <f t="shared" si="13"/>
+        <v>42577</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <f t="shared" si="13"/>
+        <v>42578</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <f t="shared" si="13"/>
+        <v>42579</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <f t="shared" si="13"/>
+        <v>42580</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3">
+        <f t="shared" si="13"/>
+        <v>42581</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <f t="shared" si="13"/>
+        <v>42582</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
+        <f t="shared" si="13"/>
+        <v>42583</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a ton of updates
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -920,6 +920,15 @@
                 <c:pt idx="92">
                   <c:v>132</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>143</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1554,6 +1563,15 @@
                 <c:pt idx="92">
                   <c:v>116</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>132</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2188,6 +2206,15 @@
                 <c:pt idx="92">
                   <c:v>116</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>132</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2822,6 +2849,15 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3454,6 +3490,15 @@
                 <c:pt idx="92">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3467,8 +3512,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223163160"/>
-        <c:axId val="223163552"/>
+        <c:axId val="171799184"/>
+        <c:axId val="171799576"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4099,6 +4144,15 @@
                 <c:pt idx="92" formatCode="General">
                   <c:v>0.87878787878787878</c:v>
                 </c:pt>
+                <c:pt idx="93" formatCode="General">
+                  <c:v>0.79720279720279719</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="General">
+                  <c:v>0.95238095238095233</c:v>
+                </c:pt>
+                <c:pt idx="95" formatCode="General">
+                  <c:v>0.92307692307692313</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4112,11 +4166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223164336"/>
-        <c:axId val="223163944"/>
+        <c:axId val="219744144"/>
+        <c:axId val="219743752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223163160"/>
+        <c:axId val="171799184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -4230,12 +4284,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223163552"/>
+        <c:crossAx val="171799576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223163552"/>
+        <c:axId val="171799576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4348,12 +4402,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223163160"/>
+        <c:crossAx val="171799184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223163944"/>
+        <c:axId val="219743752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4449,12 +4503,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223164336"/>
+        <c:crossAx val="219744144"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223164336"/>
+        <c:axId val="219744144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4464,7 +4518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223163944"/>
+        <c:crossAx val="219743752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5244,6 +5298,15 @@
                 <c:pt idx="92">
                   <c:v>46.292297979790334</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>43.209502923694487</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="0">
+                  <c:v>42.766785714841845</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>42.880429292748552</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5878,6 +5941,15 @@
                 <c:pt idx="92">
                   <c:v>35.283333335537463</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>35.250000004889444</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>35.250000004889444</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>35.200000003678724</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6512,6 +6584,15 @@
                 <c:pt idx="92">
                   <c:v>65.916666673729196</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>61.283333336468786</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="0">
+                  <c:v>57.916666658129543</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>60.399999995715916</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6525,11 +6606,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223165120"/>
-        <c:axId val="223165512"/>
+        <c:axId val="219744928"/>
+        <c:axId val="219745320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223165120"/>
+        <c:axId val="219744928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -6642,12 +6723,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223165512"/>
+        <c:crossAx val="219745320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223165512"/>
+        <c:axId val="219745320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6759,7 +6840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223165120"/>
+        <c:crossAx val="219744928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7950,7 +8031,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7961,7 +8042,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7972,7 +8053,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7999,7 +8080,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8287,8 +8368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94:J94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97:J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9994,7 +10075,7 @@
         <v>0.9642857142857143</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>42522</v>
       </c>
@@ -10026,8 +10107,11 @@
       <c r="J49" s="5">
         <v>54.966666660038754</v>
       </c>
+      <c r="K49">
+        <v>0.9726027397260274</v>
+      </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>42523</v>
       </c>
@@ -10059,8 +10143,11 @@
       <c r="J50" s="5">
         <v>57.300000004470348</v>
       </c>
+      <c r="K50">
+        <v>0.95319634703196343</v>
+      </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>42524</v>
       </c>
@@ -10092,8 +10179,11 @@
       <c r="J51" s="5">
         <v>54.883333338657394</v>
       </c>
+      <c r="K51">
+        <v>0.96561771561771548</v>
+      </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>42525</v>
       </c>
@@ -10125,8 +10215,11 @@
       <c r="J52" s="5">
         <v>63.200000000651926</v>
       </c>
+      <c r="K52">
+        <v>0.95777027027027029</v>
+      </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>42526</v>
       </c>
@@ -10158,8 +10251,11 @@
       <c r="J53" s="5">
         <v>54.3999999971129</v>
       </c>
+      <c r="K53">
+        <v>0.95578231292517002</v>
+      </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>42527</v>
       </c>
@@ -10191,8 +10287,11 @@
       <c r="J54" s="5">
         <v>64.966666671680287</v>
       </c>
+      <c r="K54">
+        <v>0.94482758620689655</v>
+      </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>42528</v>
       </c>
@@ -10224,8 +10323,11 @@
       <c r="J55" s="5">
         <v>58.450000000884756</v>
       </c>
+      <c r="K55">
+        <v>0.93055555555555558</v>
+      </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>42529</v>
       </c>
@@ -10257,8 +10359,11 @@
       <c r="J56" s="5">
         <v>59.116666666232049</v>
       </c>
+      <c r="K56">
+        <v>0.91666666666666663</v>
+      </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>42530</v>
       </c>
@@ -10290,8 +10395,11 @@
       <c r="J57" s="5">
         <v>59.699999999720603</v>
       </c>
+      <c r="K57">
+        <v>0.93221393034825872</v>
+      </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>42531</v>
       </c>
@@ -10323,8 +10431,11 @@
       <c r="J58" s="5">
         <v>59.566666666651145</v>
       </c>
+      <c r="K58">
+        <v>0.96166666666666667</v>
+      </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>42532</v>
       </c>
@@ -10356,8 +10467,11 @@
       <c r="J59" s="5">
         <v>59.566666666651145</v>
       </c>
+      <c r="K59">
+        <v>0.98582766439909308</v>
+      </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>42533</v>
       </c>
@@ -10390,8 +10504,11 @@
       <c r="J60" s="5">
         <v>62.350000001024455</v>
       </c>
+      <c r="K60">
+        <v>0.91079812206572752</v>
+      </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>42534</v>
       </c>
@@ -10424,8 +10541,11 @@
       <c r="J61" s="5">
         <v>76.250000002328306</v>
       </c>
+      <c r="K61">
+        <v>0.90653153153153165</v>
+      </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>42535</v>
       </c>
@@ -10458,8 +10578,11 @@
       <c r="J62" s="5">
         <v>79.533333338331431</v>
       </c>
+      <c r="K62">
+        <v>0.95517241379310347</v>
+      </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>42536</v>
       </c>
@@ -10492,8 +10615,11 @@
       <c r="J63" s="5">
         <v>82.933333336841315</v>
       </c>
+      <c r="K63">
+        <v>0.89786967418546371</v>
+      </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>42537</v>
       </c>
@@ -10526,8 +10652,11 @@
       <c r="J64" s="5">
         <v>52.400000001071021</v>
       </c>
+      <c r="K64">
+        <v>0.85486111111111107</v>
+      </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>42538</v>
       </c>
@@ -10560,8 +10689,11 @@
       <c r="J65" s="5">
         <v>57.866666667396203</v>
       </c>
+      <c r="K65">
+        <v>0.85486111111111107</v>
+      </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>42539</v>
       </c>
@@ -10594,8 +10726,11 @@
       <c r="J66" s="5">
         <v>62.866666673216969</v>
       </c>
+      <c r="K66">
+        <v>0.92194835680751186</v>
+      </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>42540</v>
       </c>
@@ -10628,8 +10763,11 @@
       <c r="J67" s="5">
         <v>66.58333332859911</v>
       </c>
+      <c r="K67">
+        <v>0.91608391608391604</v>
+      </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>42541</v>
       </c>
@@ -10662,8 +10800,11 @@
       <c r="J68" s="5">
         <v>54.199999992270023</v>
       </c>
+      <c r="K68">
+        <v>0.96009389671361489</v>
+      </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>42542</v>
       </c>
@@ -10696,8 +10837,11 @@
       <c r="J69" s="5">
         <v>61.383333338890225</v>
       </c>
+      <c r="K69">
+        <v>0.88260340632603396</v>
+      </c>
     </row>
-    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>42543</v>
       </c>
@@ -10730,8 +10874,11 @@
       <c r="J70" s="5">
         <v>56.366666662506759</v>
       </c>
+      <c r="K70">
+        <v>0.93838028169014087</v>
+      </c>
     </row>
-    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>42544</v>
       </c>
@@ -10762,8 +10909,11 @@
       <c r="J71" s="12">
         <v>59.249999999301508</v>
       </c>
+      <c r="K71">
+        <v>0.96276595744680848</v>
+      </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>42545</v>
       </c>
@@ -10794,8 +10944,11 @@
       <c r="J72" s="2">
         <v>56.516666666138917</v>
       </c>
+      <c r="K72">
+        <v>0.90136054421768708</v>
+      </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>42546</v>
       </c>
@@ -10826,8 +10979,11 @@
       <c r="J73" s="2">
         <v>57.866666667396203</v>
       </c>
+      <c r="K73">
+        <v>0.96270396270396286</v>
+      </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>42547</v>
       </c>
@@ -10858,8 +11014,11 @@
       <c r="J74" s="2">
         <v>61.716666676802561</v>
       </c>
+      <c r="K74">
+        <v>0.98928571428571432</v>
+      </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>42548</v>
       </c>
@@ -10890,8 +11049,11 @@
       <c r="J75" s="2">
         <v>61.716666676802561</v>
       </c>
+      <c r="K75">
+        <v>0.96759259259259267</v>
+      </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <f>A75+1</f>
         <v>42549</v>
@@ -10923,8 +11085,11 @@
       <c r="J76" s="2">
         <v>56.549999996786937</v>
       </c>
+      <c r="K76">
+        <v>0.91608391608391604</v>
+      </c>
     </row>
-    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <f t="shared" ref="A77:A110" si="13">A76+1</f>
         <v>42550</v>
@@ -10957,8 +11122,11 @@
       <c r="J77" s="2">
         <v>56.549999996786937</v>
       </c>
+      <c r="K77">
+        <v>0.96347031963470309</v>
+      </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <f t="shared" si="13"/>
         <v>42551</v>
@@ -10990,8 +11158,11 @@
       <c r="J78" s="2">
         <v>60</v>
       </c>
+      <c r="K78">
+        <v>0.98661800486618001</v>
+      </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <f t="shared" si="13"/>
         <v>42552</v>
@@ -11024,7 +11195,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <f t="shared" si="13"/>
         <v>42553</v>
@@ -11520,97 +11691,178 @@
         <v>65.916666673729196</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <f t="shared" si="13"/>
         <v>42568</v>
       </c>
+      <c r="B95">
+        <v>143</v>
+      </c>
+      <c r="C95">
+        <v>114</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>29</v>
+      </c>
+      <c r="F95">
+        <v>114</v>
+      </c>
+      <c r="G95">
+        <v>0.79720279720279719</v>
+      </c>
+      <c r="H95" s="2">
+        <v>43.209502923694487</v>
+      </c>
+      <c r="I95" s="2">
+        <v>35.250000004889444</v>
+      </c>
+      <c r="J95" s="2">
+        <v>61.283333336468786</v>
+      </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <f t="shared" si="13"/>
         <v>42569</v>
       </c>
+      <c r="B96">
+        <v>146</v>
+      </c>
+      <c r="C96">
+        <v>140</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>7</v>
+      </c>
+      <c r="F96">
+        <v>140</v>
+      </c>
+      <c r="G96">
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="H96" s="13">
+        <v>42.766785714841845</v>
+      </c>
+      <c r="I96" s="2">
+        <v>35.250000004889444</v>
+      </c>
+      <c r="J96" s="12">
+        <v>57.916666658129543</v>
+      </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <f t="shared" si="13"/>
         <v>42570</v>
       </c>
+      <c r="B97">
+        <v>143</v>
+      </c>
+      <c r="C97">
+        <v>132</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>11</v>
+      </c>
+      <c r="F97">
+        <v>132</v>
+      </c>
+      <c r="G97">
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="H97" s="2">
+        <v>42.880429292748552</v>
+      </c>
+      <c r="I97" s="2">
+        <v>35.200000003678724</v>
+      </c>
+      <c r="J97" s="2">
+        <v>60.399999995715916</v>
+      </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <f t="shared" si="13"/>
         <v>42571</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <f t="shared" si="13"/>
         <v>42572</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <f t="shared" si="13"/>
         <v>42573</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <f t="shared" si="13"/>
         <v>42574</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <f t="shared" si="13"/>
         <v>42575</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <f t="shared" si="13"/>
         <v>42576</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <f t="shared" si="13"/>
         <v>42577</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <f t="shared" si="13"/>
         <v>42578</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <f t="shared" si="13"/>
         <v>42579</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <f t="shared" si="13"/>
         <v>42580</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <f t="shared" si="13"/>
         <v>42581</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <f t="shared" si="13"/>
         <v>42582</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <f t="shared" si="13"/>
         <v>42583</v>

</xml_diff>

<commit_message>
more reports from the past few days
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Completion Stats" sheetId="2" r:id="rId2"/>
     <sheet name="Trip Length Stats" sheetId="5" r:id="rId3"/>
+    <sheet name="DE.1.0.7.0 comparisons" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -929,6 +930,12 @@
                 <c:pt idx="95">
                   <c:v>143</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>138</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1572,6 +1579,12 @@
                 <c:pt idx="95">
                   <c:v>132</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>132</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2215,6 +2228,12 @@
                 <c:pt idx="95">
                   <c:v>132</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>132</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2858,6 +2877,12 @@
                 <c:pt idx="95">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3499,6 +3524,12 @@
                 <c:pt idx="95">
                   <c:v>11</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3512,8 +3543,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="171799184"/>
-        <c:axId val="171799576"/>
+        <c:axId val="284666480"/>
+        <c:axId val="359120504"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4153,6 +4184,12 @@
                 <c:pt idx="95" formatCode="General">
                   <c:v>0.92307692307692313</c:v>
                 </c:pt>
+                <c:pt idx="96" formatCode="General">
+                  <c:v>0.93006993006993011</c:v>
+                </c:pt>
+                <c:pt idx="97" formatCode="General">
+                  <c:v>0.95652173913043481</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4166,11 +4203,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="219744144"/>
-        <c:axId val="219743752"/>
+        <c:axId val="359121288"/>
+        <c:axId val="359120896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="171799184"/>
+        <c:axId val="284666480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -4284,12 +4321,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171799576"/>
+        <c:crossAx val="359120504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171799576"/>
+        <c:axId val="359120504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4402,12 +4439,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171799184"/>
+        <c:crossAx val="284666480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="219743752"/>
+        <c:axId val="359120896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4503,12 +4540,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219744144"/>
+        <c:crossAx val="359121288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="219744144"/>
+        <c:axId val="359121288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4518,7 +4555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219743752"/>
+        <c:crossAx val="359120896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4634,6 +4671,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5307,6 +5345,12 @@
                 <c:pt idx="95">
                   <c:v>42.880429292748552</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>43.965037593896383</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>46.900252525837544</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5950,6 +5994,12 @@
                 <c:pt idx="95">
                   <c:v>35.200000003678724</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>35.333333326270804</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>34.966666668187827</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6593,6 +6643,12 @@
                 <c:pt idx="95">
                   <c:v>60.399999995715916</c:v>
                 </c:pt>
+                <c:pt idx="96">
+                  <c:v>64.599999992642552</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>107.68333333893679</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6606,11 +6662,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="219744928"/>
-        <c:axId val="219745320"/>
+        <c:axId val="359122072"/>
+        <c:axId val="359122464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="219744928"/>
+        <c:axId val="359122072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -6657,6 +6713,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6723,12 +6780,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219745320"/>
+        <c:crossAx val="359122464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="219745320"/>
+        <c:axId val="359122464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6774,6 +6831,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6840,7 +6898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219744928"/>
+        <c:crossAx val="359122072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6854,6 +6912,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8031,7 +8090,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8053,7 +8112,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -8368,8 +8427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97:J97"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="H103" sqref="H102:H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11795,36 +11854,198 @@
         <f t="shared" si="13"/>
         <v>42571</v>
       </c>
+      <c r="B98">
+        <v>143</v>
+      </c>
+      <c r="C98">
+        <v>133</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>10</v>
+      </c>
+      <c r="F98">
+        <v>133</v>
+      </c>
+      <c r="G98">
+        <v>0.93006993006993011</v>
+      </c>
+      <c r="H98" s="2">
+        <v>43.965037593896383</v>
+      </c>
+      <c r="I98" s="2">
+        <v>35.333333326270804</v>
+      </c>
+      <c r="J98" s="2">
+        <v>64.599999992642552</v>
+      </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <f t="shared" si="13"/>
         <v>42572</v>
       </c>
+      <c r="B99">
+        <v>138</v>
+      </c>
+      <c r="C99">
+        <v>132</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>6</v>
+      </c>
+      <c r="F99">
+        <v>132</v>
+      </c>
+      <c r="G99">
+        <v>0.95652173913043481</v>
+      </c>
+      <c r="H99" s="2">
+        <v>46.900252525837544</v>
+      </c>
+      <c r="I99" s="2">
+        <v>34.966666668187827</v>
+      </c>
+      <c r="J99" s="2">
+        <v>107.68333333893679</v>
+      </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <f t="shared" si="13"/>
         <v>42573</v>
       </c>
+      <c r="B100">
+        <v>140</v>
+      </c>
+      <c r="C100">
+        <v>137</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100">
+        <v>137</v>
+      </c>
+      <c r="G100">
+        <v>0.97857142857142854</v>
+      </c>
+      <c r="H100" s="2">
+        <v>42.51934306543103</v>
+      </c>
+      <c r="I100" s="2">
+        <v>34.800000004470348</v>
+      </c>
+      <c r="J100" s="2">
+        <v>55.33333332859911</v>
+      </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <f t="shared" si="13"/>
         <v>42574</v>
       </c>
+      <c r="B101">
+        <v>140</v>
+      </c>
+      <c r="C101">
+        <v>134</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>6</v>
+      </c>
+      <c r="F101">
+        <v>134</v>
+      </c>
+      <c r="G101">
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="H101" s="2">
+        <v>43.084999999655075</v>
+      </c>
+      <c r="I101" s="2">
+        <v>35.016666669398546</v>
+      </c>
+      <c r="J101" s="2">
+        <v>79.049999996786937</v>
+      </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <f t="shared" si="13"/>
         <v>42575</v>
       </c>
+      <c r="B102">
+        <v>145</v>
+      </c>
+      <c r="C102">
+        <v>143</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102">
+        <v>143</v>
+      </c>
+      <c r="G102">
+        <v>0.98620689655172411</v>
+      </c>
+      <c r="H102" s="2">
+        <v>43.229836829566771</v>
+      </c>
+      <c r="I102" s="2">
+        <v>35.416666668606922</v>
+      </c>
+      <c r="J102" s="2">
+        <v>62.133333336096257</v>
+      </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <f t="shared" si="13"/>
         <v>42576</v>
       </c>
+      <c r="B103">
+        <v>138</v>
+      </c>
+      <c r="C103">
+        <v>131</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>7</v>
+      </c>
+      <c r="F103">
+        <v>131</v>
+      </c>
+      <c r="G103">
+        <v>0.94927536231884058</v>
+      </c>
+      <c r="H103" s="2">
+        <v>44.978371500455282</v>
+      </c>
+      <c r="I103" s="2">
+        <v>36.083333323476836</v>
+      </c>
+      <c r="J103" s="2">
+        <v>64.74999999627471</v>
+      </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
@@ -11872,4 +12093,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor updates to each
</commit_message>
<xml_diff>
--- a/EC/Train Run Trends.xlsx
+++ b/EC/Train Run Trends.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EC Data" sheetId="1" r:id="rId1"/>
@@ -709,6 +709,42 @@
                 <c:pt idx="108">
                   <c:v>42583</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42585</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42586</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42587</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42588</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42589</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42590</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42591</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42592</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42593</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42594</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42595</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1031,6 +1067,24 @@
                   <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="104">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="110">
                   <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
@@ -2061,6 +2115,42 @@
                 <c:pt idx="108">
                   <c:v>42583</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42585</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42586</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42587</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42588</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42589</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42590</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42591</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42592</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42593</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42594</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42595</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2384,6 +2474,24 @@
                 </c:pt>
                 <c:pt idx="104">
                   <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2764,6 +2872,42 @@
                 <c:pt idx="108">
                   <c:v>42583</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42585</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42586</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42587</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42588</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42589</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42590</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42591</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42592</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42593</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42594</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42595</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3086,6 +3230,24 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3465,6 +3627,42 @@
                 <c:pt idx="108">
                   <c:v>42583</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42585</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42586</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42587</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42588</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42589</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42590</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42591</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42592</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42593</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42594</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42595</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3788,6 +3986,24 @@
                 </c:pt>
                 <c:pt idx="104">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3802,8 +4018,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202757544"/>
-        <c:axId val="202750880"/>
+        <c:axId val="329440712"/>
+        <c:axId val="329651200"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4179,6 +4395,42 @@
                 <c:pt idx="108">
                   <c:v>42583</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42585</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42586</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42587</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42588</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42589</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42590</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42591</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42592</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42593</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42594</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42595</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4502,6 +4754,24 @@
                 </c:pt>
                 <c:pt idx="104" formatCode="General">
                   <c:v>0.97916666666666663</c:v>
+                </c:pt>
+                <c:pt idx="105" formatCode="General">
+                  <c:v>0.97945205479452058</c:v>
+                </c:pt>
+                <c:pt idx="106" formatCode="General">
+                  <c:v>0.98630136986301364</c:v>
+                </c:pt>
+                <c:pt idx="107" formatCode="General">
+                  <c:v>0.89583333333333337</c:v>
+                </c:pt>
+                <c:pt idx="108" formatCode="General">
+                  <c:v>0.97222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="109" formatCode="General">
+                  <c:v>0.95833333333333337</c:v>
+                </c:pt>
+                <c:pt idx="110" formatCode="General">
+                  <c:v>0.95138888888888884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4516,11 +4786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202755584"/>
-        <c:axId val="202757152"/>
+        <c:axId val="329651984"/>
+        <c:axId val="329651592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202757544"/>
+        <c:axId val="329440712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -4634,12 +4904,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202750880"/>
+        <c:crossAx val="329651200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202750880"/>
+        <c:axId val="329651200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4752,12 +5022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202757544"/>
+        <c:crossAx val="329440712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202757152"/>
+        <c:axId val="329651592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4853,12 +5123,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202755584"/>
+        <c:crossAx val="329651984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202755584"/>
+        <c:axId val="329651984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4868,7 +5138,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202757152"/>
+        <c:crossAx val="329651592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4984,6 +5254,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5717,6 +5988,18 @@
                 <c:pt idx="104">
                   <c:v>43.317257683312995</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>43.175757575374732</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>43.780092592714936</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>44.854780362003893</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>44.596904762421865</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6420,6 +6703,18 @@
                 <c:pt idx="104">
                   <c:v>35.233333334326744</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>34.999999998835847</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>34.883333336329088</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>36.466666662599891</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>36.033333332743496</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7123,6 +7418,18 @@
                 <c:pt idx="104">
                   <c:v>57.933333328692243</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>64.69999999506399</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>55.833333330228925</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>65.233333337819204</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>61.750000007450581</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7136,11 +7443,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202033344"/>
-        <c:axId val="202032168"/>
+        <c:axId val="329652768"/>
+        <c:axId val="381496720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202033344"/>
+        <c:axId val="329652768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42469"/>
@@ -7187,6 +7494,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7253,12 +7561,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202032168"/>
+        <c:crossAx val="381496720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202032168"/>
+        <c:axId val="381496720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7304,6 +7612,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7370,7 +7679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202033344"/>
+        <c:crossAx val="329652768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7384,6 +7693,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7485,6 +7795,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7945,6 +8256,24 @@
                 <c:pt idx="4">
                   <c:v>47</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8315,6 +8644,24 @@
                 <c:pt idx="4">
                   <c:v>46</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8745,6 +9092,24 @@
                 <c:pt idx="4">
                   <c:v>46</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9175,6 +9540,24 @@
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9603,6 +9986,24 @@
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9616,8 +10017,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201691440"/>
-        <c:axId val="203634656"/>
+        <c:axId val="260293600"/>
+        <c:axId val="260293992"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -10044,6 +10445,24 @@
                 <c:pt idx="4">
                   <c:v>0.97872340425531912</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97872340425531912</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97297297297297303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95744680851063835</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93478260869565222</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -10057,11 +10476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202528560"/>
-        <c:axId val="282819560"/>
+        <c:axId val="259747224"/>
+        <c:axId val="259746832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201691440"/>
+        <c:axId val="260293600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42650"/>
@@ -10109,6 +10528,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10175,12 +10595,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203634656"/>
+        <c:crossAx val="260293992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203634656"/>
+        <c:axId val="260293992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10226,6 +10646,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10292,12 +10713,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201691440"/>
+        <c:crossAx val="260293600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="282819560"/>
+        <c:axId val="259746832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -10332,6 +10753,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10392,12 +10814,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202528560"/>
+        <c:crossAx val="259747224"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202528560"/>
+        <c:axId val="259747224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10407,7 +10829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282819560"/>
+        <c:crossAx val="259746832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10421,6 +10843,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10522,6 +10945,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10955,6 +11379,24 @@
                 <c:pt idx="4">
                   <c:v>19.50760869562383</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.689492753575273</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.625771605866721</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.192156863412546</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.543617020217464</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.8611111107748</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.612592593766749</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -11358,6 +11800,24 @@
                 <c:pt idx="4">
                   <c:v>14.06666666502133</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.083333338843659</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.983333329902962</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.166666667442769</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.966666662599891</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.383333332370967</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.949999995296821</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -11761,6 +12221,24 @@
                 <c:pt idx="4">
                   <c:v>37.116666657384485</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.33333333930932</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78.050000004004687</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.599999993806705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.833333331160247</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36.466666662599891</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83.133333331206813</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -11774,11 +12252,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="342583248"/>
-        <c:axId val="342583640"/>
+        <c:axId val="256660440"/>
+        <c:axId val="260321784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="342583248"/>
+        <c:axId val="256660440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42650"/>
@@ -11826,6 +12304,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11892,12 +12371,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342583640"/>
+        <c:crossAx val="260321784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="342583640"/>
+        <c:axId val="260321784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11943,6 +12422,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12009,7 +12489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342583248"/>
+        <c:crossAx val="256660440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12023,6 +12503,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14312,7 +14793,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14356,7 +14837,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664408" cy="6291513"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -14410,7 +14891,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668550" cy="6291303"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -14723,10 +15204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105:G105"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112:J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17448,7 +17929,7 @@
     </row>
     <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <f t="shared" ref="A77:A110" si="13">A76+1</f>
+        <f t="shared" ref="A77:A122" si="13">A76+1</f>
         <v>42550</v>
       </c>
       <c r="B77">
@@ -18449,23 +18930,257 @@
         <f t="shared" si="13"/>
         <v>42580</v>
       </c>
+      <c r="B107">
+        <v>146</v>
+      </c>
+      <c r="C107">
+        <v>143</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>3</v>
+      </c>
+      <c r="F107">
+        <v>143</v>
+      </c>
+      <c r="G107">
+        <v>0.97945205479452058</v>
+      </c>
+      <c r="H107" s="2">
+        <v>43.175757575374732</v>
+      </c>
+      <c r="I107" s="2">
+        <v>34.999999998835847</v>
+      </c>
+      <c r="J107" s="2">
+        <v>64.69999999506399</v>
+      </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <f t="shared" si="13"/>
         <v>42581</v>
       </c>
+      <c r="B108">
+        <v>146</v>
+      </c>
+      <c r="C108">
+        <v>144</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>2</v>
+      </c>
+      <c r="F108">
+        <v>144</v>
+      </c>
+      <c r="G108">
+        <v>0.98630136986301364</v>
+      </c>
+      <c r="H108" s="2">
+        <v>43.780092592714936</v>
+      </c>
+      <c r="I108" s="2">
+        <v>34.883333336329088</v>
+      </c>
+      <c r="J108" s="2">
+        <v>55.833333330228925</v>
+      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <f t="shared" si="13"/>
         <v>42582</v>
       </c>
+      <c r="B109">
+        <v>144</v>
+      </c>
+      <c r="C109">
+        <v>129</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>15</v>
+      </c>
+      <c r="F109">
+        <v>129</v>
+      </c>
+      <c r="G109">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="H109" s="2">
+        <v>44.854780362003893</v>
+      </c>
+      <c r="I109" s="2">
+        <v>36.466666662599891</v>
+      </c>
+      <c r="J109" s="2">
+        <v>65.233333337819204</v>
+      </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <f t="shared" si="13"/>
         <v>42583</v>
+      </c>
+      <c r="B110">
+        <v>144</v>
+      </c>
+      <c r="C110">
+        <v>140</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>4</v>
+      </c>
+      <c r="F110">
+        <v>140</v>
+      </c>
+      <c r="G110">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="H110" s="2">
+        <v>44.596904762421865</v>
+      </c>
+      <c r="I110" s="2">
+        <v>36.033333332743496</v>
+      </c>
+      <c r="J110" s="2">
+        <v>61.750000007450581</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <f t="shared" si="13"/>
+        <v>42584</v>
+      </c>
+      <c r="B111">
+        <v>144</v>
+      </c>
+      <c r="C111">
+        <v>138</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>6</v>
+      </c>
+      <c r="F111">
+        <v>138</v>
+      </c>
+      <c r="G111">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="H111" s="2">
+        <v>44.651086956424557</v>
+      </c>
+      <c r="I111" s="2">
+        <v>35.316666676662862</v>
+      </c>
+      <c r="J111" s="2">
+        <v>63.133333328878507</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <f t="shared" si="13"/>
+        <v>42585</v>
+      </c>
+      <c r="B112">
+        <v>144</v>
+      </c>
+      <c r="C112">
+        <v>137</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>7</v>
+      </c>
+      <c r="F112">
+        <v>137</v>
+      </c>
+      <c r="G112">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="H112" s="2">
+        <v>44.736131386895984</v>
+      </c>
+      <c r="I112" s="2">
+        <v>18.583333339774981</v>
+      </c>
+      <c r="J112" s="2">
+        <v>61.550000002607703</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <f t="shared" si="13"/>
+        <v>42586</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <f t="shared" si="13"/>
+        <v>42587</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <f t="shared" si="13"/>
+        <v>42588</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <f t="shared" si="13"/>
+        <v>42589</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
+        <f t="shared" si="13"/>
+        <v>42590</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
+        <f t="shared" si="13"/>
+        <v>42591</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <f t="shared" si="13"/>
+        <v>42592</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <f t="shared" si="13"/>
+        <v>42593</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <f t="shared" si="13"/>
+        <v>42594</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <f t="shared" si="13"/>
+        <v>42595</v>
       </c>
     </row>
   </sheetData>
@@ -18479,7 +19194,7 @@
   <dimension ref="A1:K119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:J6"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18700,35 +19415,197 @@
         <f t="shared" si="0"/>
         <v>42580</v>
       </c>
+      <c r="B7">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>46</v>
+      </c>
+      <c r="G7">
+        <v>0.97872340425531912</v>
+      </c>
+      <c r="H7" s="2">
+        <v>23.689492753575273</v>
+      </c>
+      <c r="I7" s="2">
+        <v>15.083333338843659</v>
+      </c>
+      <c r="J7" s="2">
+        <v>39.33333333930932</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>42581</v>
       </c>
+      <c r="B8">
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>108</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>108</v>
+      </c>
+      <c r="G8">
+        <v>0.97297297297297303</v>
+      </c>
+      <c r="H8" s="2">
+        <v>20.625771605866721</v>
+      </c>
+      <c r="I8" s="2">
+        <v>12.983333329902962</v>
+      </c>
+      <c r="J8" s="2">
+        <v>78.050000004004687</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>42582</v>
       </c>
+      <c r="B9">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>18.192156863412546</v>
+      </c>
+      <c r="I9" s="2">
+        <v>14.166666667442769</v>
+      </c>
+      <c r="J9" s="2">
+        <v>29.599999993806705</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>42583</v>
       </c>
+      <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>47</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>18.543617020217464</v>
+      </c>
+      <c r="I10" s="2">
+        <v>13.966666662599891</v>
+      </c>
+      <c r="J10" s="2">
+        <v>36.833333331160247</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>42584</v>
       </c>
+      <c r="B11">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>45</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>0.95744680851063835</v>
+      </c>
+      <c r="H11" s="2">
+        <v>20.8611111107748</v>
+      </c>
+      <c r="I11" s="2">
+        <v>14.383333332370967</v>
+      </c>
+      <c r="J11" s="2">
+        <v>36.466666662599891</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>42585</v>
+      </c>
+      <c r="B12">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>43</v>
+      </c>
+      <c r="G12">
+        <v>0.93478260869565222</v>
+      </c>
+      <c r="H12" s="2">
+        <v>21.612592593766749</v>
+      </c>
+      <c r="I12" s="2">
+        <v>14.949999995296821</v>
+      </c>
+      <c r="J12" s="2">
+        <v>83.133333331206813</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -19442,15 +20319,15 @@
       </c>
       <c r="C3" s="18">
         <f>AVERAGE('EC Data'!H102:H999)</f>
-        <v>43.904467499131201</v>
+        <v>44.119735557408355</v>
       </c>
       <c r="D3" s="18">
         <f>AVERAGE('EC Data'!I102:I999)</f>
-        <v>35.686666664667428</v>
+        <v>34.065151515480302</v>
       </c>
       <c r="E3" s="18">
         <f>AVERAGE('EC Data'!J102:J999)</f>
-        <v>61.1099999982398</v>
+        <v>61.613636363022536</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -19460,15 +20337,15 @@
       </c>
       <c r="C4" s="21">
         <f>(C3-C2)*60</f>
-        <v>44.471349700058482</v>
+        <v>57.387433196687709</v>
       </c>
       <c r="D4" s="21">
         <f t="shared" ref="D4:E4" si="0">(D3-D2)*60</f>
-        <v>51.329032122007163</v>
+        <v>-45.961876829220358</v>
       </c>
       <c r="E4" s="21">
         <f t="shared" si="0"/>
-        <v>-1.1096775408591952</v>
+        <v>29.108504346104951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>